<commit_message>
Added exception handling to AWS S3 operations.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>■概要</t>
     <rPh sb="1" eb="3">
@@ -44,25 +44,6 @@
     <t>■特記事項</t>
     <rPh sb="1" eb="5">
       <t>トッキジコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バケット名、プレフィックス、ダウンロード先のディレクトリは、ユーザーがpythonの実行画面で入力する。</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ニュウリョク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -117,25 +98,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>バケット内のディレクトリ構造(プレフィックスの構造)は、ダウンロードファイルのディレクトリ構造に反映されない。</t>
-    <rPh sb="4" eb="6">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>コウゾウ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>コウゾウ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>コウゾウ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ハンエイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>バケット名、プレフィックスは、引数で受け取る。</t>
     <rPh sb="4" eb="5">
       <t>メイ</t>
@@ -163,6 +125,89 @@
   </si>
   <si>
     <t>func_download_files</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■ツール名</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s3_object_download_tool</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・バケット内のディレクトリ構造(プレフィックスの構造)は、ダウンロードファイルのディレクトリ構造に反映されない。</t>
+    <rPh sb="5" eb="7">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・例外処理を追加。</t>
+    <rPh sb="1" eb="5">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バケット名、プレフィックス、ダウンロード先のディレクトリを、ユーザーがpythonの実行画面で入力する。</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■戻り値</t>
+    <rPh sb="1" eb="2">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>True：ダウンロード完了</t>
+    <rPh sb="11" eb="13">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>False：ClientError発生</t>
+    <rPh sb="17" eb="19">
+      <t>ハッセイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -236,13 +281,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -289,13 +334,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -358,13 +403,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -427,13 +472,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -496,13 +541,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -565,13 +610,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -639,13 +684,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -713,13 +758,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -814,13 +859,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -888,13 +933,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -941,13 +986,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1015,13 +1060,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1089,13 +1134,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1158,13 +1203,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1243,13 +1288,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1312,13 +1357,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1378,13 +1423,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1447,13 +1492,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1506,13 +1551,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1561,13 +1606,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1609,6 +1654,360 @@
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>Yes</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="2914649"/>
+          <a:ext cx="4810125" cy="5305425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="2914651"/>
+          <a:ext cx="714375" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Try</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>：</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="8401050"/>
+          <a:ext cx="4810125" cy="1143001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="正方形/長方形 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="8915400"/>
+          <a:ext cx="2743200" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>エラーログ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>で</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ClientError</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>を出力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="テキスト ボックス 23"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="8401050"/>
+          <a:ext cx="1276349" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>except ClientError</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -1921,49 +2320,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C45"/>
+  <dimension ref="B2:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B45" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C56"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -1984,42 +2343,112 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B55" t="s">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C56" t="s">
-        <v>9</v>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C68" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added authentication information and region settings, as well as branching processing for whether or not they are set.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12765"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>aws s3の指定したバケットから、指定したファイルをダウンロードする。</t>
     <rPh sb="7" eb="9">
@@ -80,6 +80,34 @@
   </si>
   <si>
     <t>バケットのフォルダ(プレフィックス)を指定してダウンロードすることができない。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■ツール名</t>
+  </si>
+  <si>
+    <t>s3_object_download_tool</t>
+  </si>
+  <si>
+    <t>アクセスキー、シークレットアクセスキー、リージョンの設定及び設定有無の分岐処理を追加。</t>
+    <rPh sb="28" eb="29">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ウム</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ブンキ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ツイカ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -153,13 +181,68 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="カギ線コネクタ 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="16" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2400300" y="5053013"/>
+          <a:ext cx="1381125" cy="3462337"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -97242"/>
+            <a:gd name="adj2" fmla="val 100138"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -206,13 +289,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -275,13 +358,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -344,13 +427,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -413,90 +496,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="685800" y="3429000"/>
-          <a:ext cx="1924049" cy="466724"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:sysClr val="window" lastClr="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>s3</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>バケットから指定したファイルをダウンロード</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -559,13 +565,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -633,13 +639,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -698,6 +704,1262 @@
             </a:rPr>
             <a:t>終了</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685801" y="2228851"/>
+          <a:ext cx="3429000" cy="3771900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76202</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685801" y="2228852"/>
+          <a:ext cx="714375" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Try</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>：</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685801" y="6000750"/>
+          <a:ext cx="3429000" cy="971551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="6343650"/>
+          <a:ext cx="2057400" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>エラーログ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>で</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ClientError</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>を出力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="テキスト ボックス 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="6000750"/>
+          <a:ext cx="1276349" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>except ClientError</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="フローチャート: 判断 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="4629150"/>
+          <a:ext cx="2752725" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>アクセスキー、シークレットアクセスキー、リージョンの設定</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="5514975"/>
+          <a:ext cx="800100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>設定する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3771899" y="4752975"/>
+          <a:ext cx="1743076" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>設定しない</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
+            <a:t> or </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>無効な入力</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="正方形/長方形 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="5829300"/>
+          <a:ext cx="2057400" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>アクセスキーを入力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="正方形/長方形 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="6219825"/>
+          <a:ext cx="2057400" cy="466724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>s3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>バケットからファイルをダウンロード</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="正方形/長方形 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="6343650"/>
+          <a:ext cx="2057400" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>シークレットアクセスキーを入力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="正方形/長方形 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="6858000"/>
+          <a:ext cx="2057400" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>リージョンを入力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="正方形/長方形 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="7372349"/>
+          <a:ext cx="2057400" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>アクセスキー、シークレットアクセスキー、リージョンを指定し、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>s3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>バケットからファイルをダウンロード</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>159328</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="正方形/長方形 28"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="10448925"/>
+          <a:ext cx="2057400" cy="511753"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>一時停止</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>何かキーを押すまで実行画面を表示</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="フローチャート: 判断 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3752850" y="5314950"/>
+          <a:ext cx="2752725" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>無効な入力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="テキスト ボックス 25"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5191125" y="5848350"/>
+          <a:ext cx="800100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="カギ線コネクタ 26"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="25" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2400300" y="4629150"/>
+          <a:ext cx="4105275" cy="1109663"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -5568"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="テキスト ボックス 30"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="5772150"/>
+          <a:ext cx="800100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1008,7 +2270,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C37"/>
+  <dimension ref="B2:C74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1016,32 +2278,47 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C4" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B6" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B36" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B72" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C37" t="s">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C73" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C74" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes have been made to the file download process.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -188,7 +188,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -199,13 +199,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2400300" y="5053013"/>
-          <a:ext cx="1381125" cy="3462337"/>
+          <a:off x="2400300" y="5224463"/>
+          <a:ext cx="1381125" cy="3357562"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -97242"/>
-            <a:gd name="adj2" fmla="val 100138"/>
+            <a:gd name="adj1" fmla="val -96552"/>
+            <a:gd name="adj2" fmla="val 100000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -242,7 +242,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -496,13 +496,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -639,13 +639,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -719,7 +719,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -841,13 +841,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -905,13 +905,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1006,13 +1006,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1396,7 +1396,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>バケットからファイルをダウンロード</a:t>
+            <a:t>インスタンスを作成</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1551,8 +1551,8 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1561,8 +1561,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="7372349"/>
-          <a:ext cx="2057400" cy="847725"/>
+          <a:off x="1371600" y="7543799"/>
+          <a:ext cx="2057400" cy="857251"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1619,7 +1619,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>バケットからファイルをダウンロード</a:t>
+            <a:t>インスタンスを作成</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1630,13 +1630,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>159328</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1960,6 +1960,83 @@
             <a:t>Yes</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="正方形/長方形 27"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="8743950"/>
+          <a:ext cx="2057400" cy="857251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>s3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>バケットからファイルをダウンロード</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2270,7 +2347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C74"/>
+  <dimension ref="B2:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2306,18 +2383,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B72" t="s">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B76" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C73" t="s">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C77" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C74" t="s">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C78" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added function func_download_files. Left the implementation of the function call pending.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="func_download_files" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>aws s3の指定したバケットから、指定したファイルをダウンロードする。</t>
     <rPh sb="7" eb="9">
@@ -106,6 +107,126 @@
       <t>ショリ</t>
     </rPh>
     <rPh sb="40" eb="42">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■関数名</t>
+    <rPh sb="1" eb="3">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>func_download_files</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aws s3の指定したバケット内の、指定したプレフィックスを持つファイルを全てダウンロードする。</t>
+    <rPh sb="7" eb="9">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>スベ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バケット名、プレフィックスは、引数で受け取る。</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■引数</t>
+    <rPh sb="1" eb="3">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バケット名</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プレフィックス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■戻り値</t>
+    <rPh sb="1" eb="2">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>True：ダウンロード完了</t>
+    <rPh sb="11" eb="13">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>False：ClientError発生</t>
+    <rPh sb="17" eb="19">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・バケット内のディレクトリ構造(プレフィックスの構造)は、ダウンロードファイルのディレクトリ構造に反映されない。</t>
+    <rPh sb="5" eb="7">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ハンエイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・例外処理を追加。</t>
+    <rPh sb="1" eb="5">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
       <t>ツイカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -2037,6 +2158,1097 @@
             </a:rPr>
             <a:t>バケットからファイルをダウンロード</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="直線コネクタ 1"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2743200" y="3419475"/>
+          <a:ext cx="1" cy="6867525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="フローチャート: 端子 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371601" y="3057525"/>
+          <a:ext cx="2743199" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>開始</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="フローチャート: 端子 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="10287000"/>
+          <a:ext cx="2743200" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartTerminator">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>終了</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="3943350"/>
+          <a:ext cx="2743200" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>指定したバケット内の、指定したプレフィックスを持つファイルのリストを取得する。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="片側の 2 つの角を切り取った四角形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="4800600"/>
+          <a:ext cx="2752725" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ファイルのダウンロード処理</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>終了条件：指定したプレフィックスを持つ全ファイルのダウンロード完了</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="7200900"/>
+          <a:ext cx="2743200" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>指定したプレフィックスを持つファイルを１つダウンロード</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="片側の 2 つの角を切り取った四角形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="1371599" y="8401050"/>
+          <a:ext cx="2752725" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip2SameRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="フローチャート: 判断 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="5829300"/>
+          <a:ext cx="2752725" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ダウンロードの対象は、ディレクトリか？</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2819400" y="6715125"/>
+          <a:ext cx="800100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>No</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="カギ線コネクタ 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2743200" y="6253163"/>
+          <a:ext cx="1381125" cy="1928812"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -49655"/>
+            <a:gd name="adj2" fmla="val 100000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="5953125"/>
+          <a:ext cx="800100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Yes</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="3600449"/>
+          <a:ext cx="4810125" cy="5476875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="テキスト ボックス 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="3600451"/>
+          <a:ext cx="714375" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Try</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>：</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="正方形/長方形 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="9086850"/>
+          <a:ext cx="4810125" cy="971551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="正方形/長方形 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="9429750"/>
+          <a:ext cx="2743200" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>エラーログ</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>で</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ClientError</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>を出力</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="9086850"/>
+          <a:ext cx="1276349" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>except ClientError</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2403,4 +3615,94 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
The following changes have been made. -Fixed the display of input comments -Fixed the description of the design document -Fixed a bug that prevented files with prefixes from being downloaded when downloading a single specified file
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -25,39 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>aws s3の指定したバケットから、指定したファイルをダウンロードする。</t>
-    <rPh sb="7" eb="9">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>シテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バケット名、ファイル名、ダウンロード先のディレクトリは、ユーザーがpythonの実行画面で入力する。</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>■概要</t>
     <rPh sb="1" eb="3">
@@ -259,6 +227,64 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>・s3バケットのサブフォルダ内のファイルがダウンロードできない不具合を修正。</t>
+    <rPh sb="14" eb="16">
+      <t>ナイn</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>フグアイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aws s3の指定したバケットから、指定したキーのファイルをダウンロードする。</t>
+    <rPh sb="7" eb="9">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>また、プレフィックスを指定することで、指定したプレフィックスを持つキーのファイルを全てダウンロードする。</t>
+    <rPh sb="11" eb="13">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>スベ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バケット名、s3バケット内のダウンロードファイルのキー、プレフィックス、ダウンロード先のローカルディレクトリは、ユーザーがpythonの実行画面で入力する。</t>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -330,13 +356,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>23814</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>114303</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -382,13 +408,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -437,13 +463,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -490,13 +516,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -559,13 +585,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -612,12 +638,20 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>s3</a:t>
+          </a:r>
+          <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ファイル名を入力</a:t>
+            <a:t>バケット内のダウンロードファイルのキーを入力</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -628,13 +662,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -697,13 +731,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -771,13 +805,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -845,13 +879,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -909,13 +943,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -973,13 +1007,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1042,13 +1076,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1100,13 +1134,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1167,13 +1201,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1236,13 +1270,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1313,13 +1347,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1382,13 +1416,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1451,13 +1485,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1536,13 +1570,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>159328</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1634,13 +1668,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1727,13 +1761,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1786,13 +1820,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1840,13 +1874,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1899,13 +1933,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1976,13 +2010,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2050,13 +2084,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2109,13 +2143,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2168,13 +2202,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2223,13 +2257,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2292,13 +2326,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2361,13 +2395,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2430,13 +2464,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2531,13 +2565,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2600,13 +2634,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2669,13 +2703,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2728,13 +2762,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2782,13 +2816,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2841,13 +2875,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2910,13 +2944,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2974,13 +3008,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3075,13 +3109,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3139,13 +3173,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3221,13 +3255,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3326,6 +3360,83 @@
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="正方形/長方形 46"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="11144250"/>
+          <a:ext cx="2057400" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>s3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>バケット内のダウンロードファイルのキーからファイル名を取得</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6115,7 +6226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C85"/>
+  <dimension ref="B2:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6123,47 +6234,57 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
-        <v>3</v>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B89" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B83" t="s">
-        <v>4</v>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C90" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C84" t="s">
-        <v>20</v>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C91" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C85" t="s">
-        <v>21</v>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C92" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -6183,82 +6304,82 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C91" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C92" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C93" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prerequisites to the design document.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>■概要</t>
     <rPh sb="1" eb="3">
@@ -285,6 +285,27 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>■前提条件</t>
+    <rPh sb="1" eb="5">
+      <t>ゼンテイジョウケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>python 3.10がインストールされていること。(その他のpythonバージョンでは、動作確認未実施)</t>
+    <rPh sb="45" eb="49">
+      <t>ドウサカクニン</t>
+    </rPh>
+    <rPh sb="49" eb="52">
+      <t>ミジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>awsのpython SDKであるboto3がインストールされていること。(boto3のインストールコマンド: python -m pip install boto3)</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -356,13 +377,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>23814</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>114303</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -408,13 +429,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -463,13 +484,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -516,13 +537,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -585,13 +606,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -662,13 +683,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -731,13 +752,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -805,13 +826,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -879,13 +900,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -943,13 +964,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1007,13 +1028,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1076,13 +1097,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1134,13 +1155,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1201,13 +1222,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1270,13 +1291,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1347,13 +1368,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1416,13 +1437,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1485,13 +1506,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1570,13 +1591,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>159328</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1668,13 +1689,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1761,13 +1782,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1820,13 +1841,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1874,13 +1895,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1933,13 +1954,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2010,13 +2031,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2084,13 +2105,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2143,13 +2164,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2202,13 +2223,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>79</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2257,13 +2278,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2326,13 +2347,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2395,13 +2416,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2464,13 +2485,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2565,13 +2586,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2634,13 +2655,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2703,13 +2724,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2762,13 +2783,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2816,13 +2837,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2875,13 +2896,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2944,13 +2965,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3008,13 +3029,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3109,13 +3130,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3173,13 +3194,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3255,13 +3276,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3369,13 +3390,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6226,7 +6247,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C92"/>
+  <dimension ref="B2:C96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6264,26 +6285,41 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B89" t="s">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B93" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C90" t="s">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C94" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C91" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C95" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C92" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C96" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added prerepuistes to the design document.
</commit_message>
<xml_diff>
--- a/設計書(s3_object_download_tool).xlsx
+++ b/設計書(s3_object_download_tool).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>■概要</t>
     <rPh sb="1" eb="3">
@@ -65,41 +65,6 @@
   </si>
   <si>
     <t>func_download_files</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>aws s3の指定したバケット内の、指定したプレフィックスを持つファイルを全てダウンロードする。</t>
-    <rPh sb="7" eb="9">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>シテイ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>スベ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バケット名、プレフィックスは、引数で受け取る。</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒキスウ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ト</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -241,19 +206,101 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>aws s3の指定したバケットから、指定したキーのファイルをダウンロードする。</t>
-    <rPh sb="7" eb="9">
+    <t>■前提条件</t>
+    <rPh sb="1" eb="5">
+      <t>ゼンテイジョウケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・aws s3の指定したバケットから、指定したキーのファイルをダウンロードする。</t>
+    <rPh sb="8" eb="10">
       <t>シテイ</t>
     </rPh>
-    <rPh sb="18" eb="20">
+    <rPh sb="19" eb="21">
       <t>シテイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>また、プレフィックスを指定することで、指定したプレフィックスを持つキーのファイルを全てダウンロードする。</t>
-    <rPh sb="11" eb="13">
+    <t>・バケット名、s3バケット内のダウンロードファイルのキー、プレフィックス、ダウンロード先のローカルディレクトリは、ユーザーがpythonの実行画面で入力する。</t>
+    <rPh sb="5" eb="6">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・aws s3の認証情報、バケットのリージョン設定の参照先は、実行環境に依存する。</t>
+    <rPh sb="8" eb="12">
+      <t>ニンショウジョウホウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="26" eb="29">
+      <t>サンショウサキ</t>
+    </rPh>
+    <rPh sb="31" eb="35">
+      <t>ジッコウカンキョウ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>イゾン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 本ツールの実行時に認証情報、バケットのリージョンを設定する場合は、iamユーザーのアクセスキー・シークレットアクセスキー、バケットのリージョンを入力する。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> また、プレフィックスを指定することで、指定したプレフィックスを持つキーのファイルを全てダウンロードする。</t>
+    <rPh sb="12" eb="14">
       <t>シテイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>スベ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・python 3.10がインストールされていること。(その他のpythonバージョンでは、動作確認未実施)</t>
+    <rPh sb="46" eb="50">
+      <t>ドウサカクニン</t>
+    </rPh>
+    <rPh sb="50" eb="53">
+      <t>ミジッシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・awsのpython SDKであるboto3がインストールされていること。(boto3のインストールコマンド: python -m pip install boto3)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・aws s3の指定したバケット内の、指定したプレフィックスを持つファイルを全てダウンロードする。</t>
+    <rPh sb="8" eb="10">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ナイ</t>
     </rPh>
     <rPh sb="19" eb="21">
       <t>シテイ</t>
@@ -261,49 +308,9 @@
     <rPh sb="31" eb="32">
       <t>モ</t>
     </rPh>
-    <rPh sb="41" eb="42">
+    <rPh sb="38" eb="39">
       <t>スベ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バケット名、s3バケット内のダウンロードファイルのキー、プレフィックス、ダウンロード先のローカルディレクトリは、ユーザーがpythonの実行画面で入力する。</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>サキ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>■前提条件</t>
-    <rPh sb="1" eb="5">
-      <t>ゼンテイジョウケン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>python 3.10がインストールされていること。(その他のpythonバージョンでは、動作確認未実施)</t>
-    <rPh sb="45" eb="49">
-      <t>ドウサカクニン</t>
-    </rPh>
-    <rPh sb="49" eb="52">
-      <t>ミジッシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>awsのpython SDKであるboto3がインストールされていること。(boto3のインストールコマンド: python -m pip install boto3)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -377,13 +384,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>23814</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>114303</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -429,13 +436,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -484,13 +491,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -537,13 +544,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -606,13 +613,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -683,13 +690,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -752,13 +759,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -826,13 +833,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -900,13 +907,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -964,13 +971,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1028,13 +1035,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1097,13 +1104,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1155,13 +1162,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1222,13 +1229,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1291,13 +1298,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1368,13 +1375,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1437,13 +1444,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1506,13 +1513,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1591,13 +1598,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>159328</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1689,13 +1696,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1782,13 +1789,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1841,13 +1848,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1895,13 +1902,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1954,13 +1961,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2031,13 +2038,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2105,13 +2112,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2164,13 +2171,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2223,13 +2230,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2278,13 +2285,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2347,13 +2354,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2416,13 +2423,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2485,13 +2492,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2586,13 +2593,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2655,13 +2662,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2724,13 +2731,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2783,13 +2790,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2837,13 +2844,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2896,13 +2903,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2965,13 +2972,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3029,13 +3036,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3130,13 +3137,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3194,13 +3201,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3276,13 +3283,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3390,13 +3397,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3472,13 +3479,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>4764</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3522,13 +3529,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3575,13 +3582,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3649,13 +3656,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3723,13 +3730,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3792,13 +3799,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3877,13 +3884,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3946,13 +3953,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4012,13 +4019,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4081,13 +4088,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4140,13 +4147,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>80963</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4195,13 +4202,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4254,13 +4261,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4318,13 +4325,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4382,13 +4389,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>166688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4437,13 +4444,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4506,13 +4513,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4564,13 +4571,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4631,13 +4638,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4700,13 +4707,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4777,13 +4784,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4846,13 +4853,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4915,13 +4922,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5000,13 +5007,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5098,13 +5105,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5157,13 +5164,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5209,13 +5216,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5268,13 +5275,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5354,13 +5361,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5447,13 +5454,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5511,13 +5518,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>661987</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>661987</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5612,13 +5619,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5676,13 +5683,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5758,13 +5765,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>661987</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>661987</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5832,13 +5839,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6247,7 +6254,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C96"/>
+  <dimension ref="B2:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6270,69 +6277,80 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B10" t="s">
-        <v>24</v>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C11" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C12" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B93" t="s">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B95" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C94" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C95" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C96" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C97" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C98" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C93"/>
+  <dimension ref="B2:C92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6355,67 +6373,62 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C7" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C11" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B90" t="s">
-        <v>2</v>
+      <c r="C90" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C92" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="C93" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>